<commit_message>
Implement Excel export functionality and backup/restore mechanism; update main script to handle email processing and error rollback.
</commit_message>
<xml_diff>
--- a/output/extracted_data.xlsx
+++ b/output/extracted_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,103 +424,90 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>NrComClient</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PretPropusClient</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>CodInitialComClient</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>CantInitialaComClient</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>NrComClient</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CodInitialComClient</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>20250628104637</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>17.22</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>LR067042</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>20250628104637</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>20250628124037</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>30735186</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>20250628124037</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>30735186</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>20250628123337</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>59.29</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>281132S0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>20250628123337</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>20250628104637</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>20250628124037</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>30735186</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>20250628123337</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>